<commit_message>
Added CAPES - BJT project to norberto's profile.
</commit_message>
<xml_diff>
--- a/database/projetos.xlsx
+++ b/database/projetos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="1300" windowWidth="24740" windowHeight="12320" activeTab="1"/>
+    <workbookView xWindow="12420" yWindow="5980" windowWidth="24740" windowHeight="12320"/>
   </bookViews>
   <sheets>
     <sheet name="norberto" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="124">
   <si>
     <t>Tipo</t>
   </si>
@@ -147,9 +147,6 @@
     <t>E_13 - APOIO A PROGRAMAS DE PÓS-GRADUAÇÃO STRICTO SENSU EM UNIVERSIDADES ESTADUAIS - 2011</t>
   </si>
   <si>
-    <t> 80.002,00</t>
-  </si>
-  <si>
     <t>E-26/110.726/2012</t>
   </si>
   <si>
@@ -385,13 +382,32 @@
   </si>
   <si>
     <t>Europe_Union</t>
+  </si>
+  <si>
+    <t>CAPES</t>
+  </si>
+  <si>
+    <t>Sistema de Simulação Numérica de Escoamentos Multifásicos</t>
+  </si>
+  <si>
+    <t> 80,002.00</t>
+  </si>
+  <si>
+    <t>067/2013</t>
+  </si>
+  <si>
+    <t>Atração de Jovens Talentos - Ciência Sem Frontreias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atração de Jovens Talentos do Programa Ciência Sem Frontreias
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,6 +429,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -498,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -561,6 +582,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -887,22 +909,22 @@
   <sheetData>
     <row r="1" spans="1:11" s="16" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>79</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>1</v>
@@ -911,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>3</v>
@@ -946,7 +968,7 @@
         <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J2" s="9">
         <v>4052348.51</v>
@@ -957,10 +979,10 @@
     </row>
     <row r="3" spans="1:11" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -978,10 +1000,10 @@
         <v>41603</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J3" s="9">
         <v>3285690</v>
@@ -1016,7 +1038,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J4" s="9">
         <v>49889.2</v>
@@ -1051,7 +1073,7 @@
         <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J5" s="9">
         <v>50000</v>
@@ -1086,7 +1108,7 @@
         <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J6" s="9">
         <v>150000</v>
@@ -1097,13 +1119,13 @@
     </row>
     <row r="7" spans="1:11" ht="56" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="17">
         <v>2012</v>
@@ -1118,10 +1140,10 @@
         <v>41672</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J7" s="9">
         <v>26834.97</v>
@@ -1132,13 +1154,13 @@
     </row>
     <row r="8" spans="1:11" ht="42" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="17">
         <v>2012</v>
@@ -1153,10 +1175,10 @@
         <v>41983</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="9">
         <v>149916.98000000001</v>
@@ -1191,7 +1213,7 @@
         <v>17</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J9" s="9">
         <v>117158</v>
@@ -1223,10 +1245,10 @@
         <v>39765</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J10" s="9">
         <v>299798</v>
@@ -1261,7 +1283,7 @@
         <v>20</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J11" s="9">
         <v>329904.90999999997</v>
@@ -1293,10 +1315,10 @@
         <v>40043</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J12" s="9">
         <v>152998</v>
@@ -1331,7 +1353,7 @@
         <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" s="9">
         <v>80000</v>
@@ -1363,10 +1385,10 @@
         <v>40183</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J14" s="9">
         <v>30000</v>
@@ -1398,10 +1420,10 @@
         <v>40814</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J15" s="9">
         <v>30000</v>
@@ -1436,7 +1458,7 @@
         <v>27</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J16" s="9">
         <v>249807.35999999999</v>
@@ -1471,7 +1493,7 @@
         <v>30</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17" s="9">
         <v>86400</v>
@@ -1503,10 +1525,10 @@
         <v>41090</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J18" s="9">
         <v>200000</v>
@@ -1538,10 +1560,10 @@
         <v>40760</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J19" s="9">
         <v>49811.56</v>
@@ -1573,10 +1595,10 @@
         <v>41243</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J20" s="10" t="s">
         <v>36</v>
@@ -1611,10 +1633,10 @@
         <v>38</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="K21" s="9">
         <v>58000</v>
@@ -1622,7 +1644,7 @@
     </row>
     <row r="22" spans="1:11" ht="42" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>15</v>
@@ -1643,10 +1665,10 @@
         <v>42135</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J22" s="9">
         <v>699014.57</v>
@@ -1657,7 +1679,7 @@
     </row>
     <row r="23" spans="1:11" ht="42" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>15</v>
@@ -1678,10 +1700,10 @@
         <v>41817</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J23" s="9">
         <v>399966.31</v>
@@ -1690,44 +1712,44 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="42" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="56" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>118</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="D24" s="17">
         <v>2013</v>
       </c>
       <c r="E24" s="17">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="F24" s="18">
-        <v>41466</v>
+        <v>41616</v>
       </c>
       <c r="G24" s="18">
-        <v>41665</v>
+        <v>42346</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>70</v>
+        <v>122</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="J24" s="9">
-        <v>399828.18</v>
+        <v>23718.14</v>
       </c>
       <c r="K24" s="9">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="56" x14ac:dyDescent="0.2">
+        <v>23718.14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="42" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>15</v>
@@ -1739,113 +1761,148 @@
         <v>2013</v>
       </c>
       <c r="E25" s="17">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="F25" s="18">
-        <v>41508</v>
+        <v>41466</v>
       </c>
       <c r="G25" s="18">
-        <v>42553</v>
+        <v>41665</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J25" s="9">
-        <v>289781.65999999997</v>
+        <v>399828.18</v>
       </c>
       <c r="K25" s="9">
-        <v>150722.66999999998</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>49</v>
+      <c r="A26" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="D26" s="17">
         <v>2013</v>
       </c>
       <c r="E26" s="17">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="F26" s="18">
-        <v>41465</v>
+        <v>41508</v>
       </c>
       <c r="G26" s="18">
-        <v>41829</v>
+        <v>42553</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J26" s="9">
-        <v>19020.59</v>
+        <v>289781.65999999997</v>
       </c>
       <c r="K26" s="9">
-        <v>19020.59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+        <v>150722.66999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="56" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="D27" s="17">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="E27" s="17">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="F27" s="18">
-        <v>42583</v>
+        <v>41465</v>
       </c>
       <c r="G27" s="18">
-        <v>43311</v>
+        <v>41829</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>116</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J27" s="9">
+        <v>19020.59</v>
+      </c>
+      <c r="K27" s="9">
+        <v>19020.59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="17">
+        <v>2015</v>
+      </c>
+      <c r="E28" s="17">
+        <v>2017</v>
+      </c>
+      <c r="F28" s="18">
+        <v>42583</v>
+      </c>
+      <c r="G28" s="18">
+        <v>43311</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J28" s="9">
         <v>2266180.4500000002</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K28" s="9">
         <v>1982400</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="12">
-        <f>SUM(K2:K27)</f>
-        <v>9820086.7300000004</v>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="12">
+        <f>SUM(K2:K28)</f>
+        <v>9843804.870000001</v>
       </c>
     </row>
   </sheetData>
@@ -1858,7 +1915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1878,22 +1935,22 @@
   <sheetData>
     <row r="1" spans="1:11" s="16" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>79</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>1</v>
@@ -1902,7 +1959,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>3</v>
@@ -1913,13 +1970,13 @@
     </row>
     <row r="2" spans="1:11" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2">
         <v>2014</v>
@@ -1934,21 +1991,21 @@
         <v>42683</v>
       </c>
       <c r="H2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" t="s">
         <v>96</v>
-      </c>
-      <c r="I2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="42" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1969,16 +2026,16 @@
         <v>42721</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" t="s">
         <v>99</v>
-      </c>
-      <c r="K3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="42" x14ac:dyDescent="0.2">
@@ -1986,10 +2043,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <v>2015</v>
@@ -2004,16 +2061,16 @@
         <v>42369</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J4" t="s">
+        <v>101</v>
+      </c>
+      <c r="K4" t="s">
         <v>102</v>
-      </c>
-      <c r="K4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2021,10 +2078,10 @@
         <v>294905</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5">
         <v>2015</v>
@@ -2039,16 +2096,16 @@
         <v>42459</v>
       </c>
       <c r="H5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new projetcs of 2016.
</commit_message>
<xml_diff>
--- a/database/projetos.xlsx
+++ b/database/projetos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="5980" windowWidth="24740" windowHeight="12320"/>
+    <workbookView xWindow="13580" yWindow="8220" windowWidth="24740" windowHeight="12320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="norberto" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="130">
   <si>
     <t>Tipo</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>E-26/010.001695/2015</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>STAL Sistema de Tratamento e Descontaminação de Água de Lastro</t>
@@ -401,6 +398,27 @@
   <si>
     <t xml:space="preserve">Atração de Jovens Talentos do Programa Ciência Sem Frontreias
 </t>
+  </si>
+  <si>
+    <t>Bolsa de Inovação Tecnológica</t>
+  </si>
+  <si>
+    <t>INT - Bolsa de Inovação Tecnológica 2016/01</t>
+  </si>
+  <si>
+    <t>E-26/000.000.000/2016</t>
+  </si>
+  <si>
+    <t>19.200,00</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de um sistema compacto e modular para o tratamento de efluentes residuais baseado em tecnologias inovadoras</t>
+  </si>
+  <si>
+    <t>25.200,00</t>
+  </si>
+  <si>
+    <t>Redução de custos operacionais e ambientais em sistema de geração termoelétrica</t>
   </si>
 </sst>
 </file>
@@ -450,7 +468,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -474,37 +492,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -515,11 +502,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -530,59 +530,76 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -887,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -902,48 +919,48 @@
     <col min="6" max="6" width="10.5" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" style="2" customWidth="1"/>
     <col min="8" max="9" width="31.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="16" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+      <c r="A2" s="4">
         <v>15283</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -952,33 +969,33 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="12">
         <v>2005</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="12">
         <v>2008</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="13">
         <v>38358</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="13">
         <v>39604</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" s="9">
+        <v>75</v>
+      </c>
+      <c r="J2" s="6">
         <v>4052348.51</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="6">
         <v>3841688.51</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -987,33 +1004,33 @@
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="12">
         <v>2010</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="12">
         <v>2013</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="13">
         <v>40507</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="13">
         <v>41603</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="9">
+        <v>55</v>
+      </c>
+      <c r="J3" s="6">
         <v>3285690</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="6">
         <v>1056090</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="28" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1022,33 +1039,33 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="12">
         <v>2006</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="12">
         <v>2008</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="13">
         <v>38868</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="13">
         <v>39599</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="9">
+        <v>56</v>
+      </c>
+      <c r="J4" s="6">
         <v>49889.2</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="6">
         <v>45889.2</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1057,33 +1074,33 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="12">
         <v>2009</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="12">
         <v>2011</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="13">
         <v>40118</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="13">
         <v>40847</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="9">
+        <v>56</v>
+      </c>
+      <c r="J5" s="6">
         <v>50000</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="6">
         <v>35000</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1092,28 +1109,28 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="12">
         <v>2012</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="12">
         <v>2014</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="13">
         <v>40913</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="13">
         <v>41644</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J6" s="9">
+        <v>104</v>
+      </c>
+      <c r="J6" s="6">
         <v>150000</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="6">
         <v>150000</v>
       </c>
     </row>
@@ -1127,33 +1144,33 @@
       <c r="C7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="12">
         <v>2012</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="12">
         <v>2014</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="13">
         <v>41158</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="13">
         <v>41672</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" s="9">
+        <v>57</v>
+      </c>
+      <c r="J7" s="6">
         <v>26834.97</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="6">
         <v>26834.97</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1162,33 +1179,33 @@
       <c r="C8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="12">
         <v>2012</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="12">
         <v>2014</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="13">
         <v>41254</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="13">
         <v>41983</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="9">
+        <v>58</v>
+      </c>
+      <c r="J8" s="6">
         <v>149916.98000000001</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="6">
         <v>149916.98000000001</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1197,33 +1214,33 @@
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="12">
         <v>2007</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="12">
         <v>2008</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="13">
         <v>39360</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="13">
         <v>39726</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" s="9">
+        <v>59</v>
+      </c>
+      <c r="J9" s="6">
         <v>117158</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="6">
         <v>50000</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1232,33 +1249,33 @@
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="12">
         <v>2007</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="12">
         <v>2008</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="13">
         <v>39399</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="13">
         <v>39765</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J10" s="9">
+        <v>59</v>
+      </c>
+      <c r="J10" s="6">
         <v>299798</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="6">
         <v>299798</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1267,33 +1284,33 @@
       <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="12">
         <v>2008</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="12">
         <v>2011</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="13">
         <v>39741</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="13">
         <v>40708</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="9">
+        <v>59</v>
+      </c>
+      <c r="J11" s="6">
         <v>329904.90999999997</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="6">
         <v>329904.90999999997</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1302,33 +1319,33 @@
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="12">
         <v>2008</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="12">
         <v>2009</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="13">
         <v>39678</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="13">
         <v>40043</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="9">
+        <v>72</v>
+      </c>
+      <c r="J12" s="6">
         <v>152998</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="6">
         <v>145798</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1337,33 +1354,33 @@
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="12">
         <v>2008</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="12">
         <v>2009</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="13">
         <v>39646</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="13">
         <v>40103</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="9">
+        <v>73</v>
+      </c>
+      <c r="J13" s="6">
         <v>80000</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="6">
         <v>61650</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1372,33 +1389,33 @@
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="12">
         <v>2009</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="12">
         <v>2010</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="13">
         <v>40091</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="13">
         <v>40183</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J14" s="9">
+        <v>74</v>
+      </c>
+      <c r="J14" s="6">
         <v>30000</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="6">
         <v>17000</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="28" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1407,33 +1424,33 @@
       <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="12">
         <v>2010</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="12">
         <v>2011</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="13">
         <v>40449</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="13">
         <v>40814</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="9">
+        <v>60</v>
+      </c>
+      <c r="J15" s="6">
         <v>30000</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="6">
         <v>20000</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="28" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1442,33 +1459,33 @@
       <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="12">
         <v>2010</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="12">
         <v>2013</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="13">
         <v>40423</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="13">
         <v>41379</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J16" s="9">
+        <v>61</v>
+      </c>
+      <c r="J16" s="6">
         <v>249807.35999999999</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="6">
         <v>173972.9</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="28" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1477,33 +1494,33 @@
       <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="12">
         <v>2010</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="12">
         <v>2013</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="13">
         <v>40347</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="13">
         <v>41486</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J17" s="9">
+        <v>56</v>
+      </c>
+      <c r="J17" s="6">
         <v>86400</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="6">
         <v>86400</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="70" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1512,33 +1529,33 @@
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="12">
         <v>2010</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="12">
         <v>2012</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="13">
         <v>40528</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="13">
         <v>41090</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="9">
+        <v>62</v>
+      </c>
+      <c r="J18" s="6">
         <v>200000</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="6">
         <v>200000</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="28" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1547,33 +1564,33 @@
       <c r="C19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="12">
         <v>2011</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="12">
         <v>2011</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="13">
         <v>40665</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="13">
         <v>40760</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J19" s="9">
+        <v>63</v>
+      </c>
+      <c r="J19" s="6">
         <v>49811.56</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="6">
         <v>15000</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="28" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1582,33 +1599,33 @@
       <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="12">
         <v>2011</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="12">
         <v>2012</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="13">
         <v>40813</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="13">
         <v>41243</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J20" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="6">
         <v>35000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:11" ht="56" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1617,33 +1634,33 @@
       <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="12">
         <v>2011</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="12">
         <v>2013</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="13">
         <v>40886</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="13">
         <v>41332</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="K21" s="9">
+        <v>65</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="K21" s="6">
         <v>58000</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1652,33 +1669,33 @@
       <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="12">
         <v>2012</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="12">
         <v>2015</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="13">
         <v>41040</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="13">
         <v>42135</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="9">
+        <v>66</v>
+      </c>
+      <c r="J22" s="6">
         <v>699014.57</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="6">
         <v>420000</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1687,68 +1704,68 @@
       <c r="C23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="12">
         <v>2012</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="12">
         <v>2014</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="13">
         <v>41087</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="13">
         <v>41817</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J23" s="9">
+        <v>67</v>
+      </c>
+      <c r="J23" s="6">
         <v>399966.31</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="6">
         <v>250000</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="12">
+        <v>2013</v>
+      </c>
+      <c r="E24" s="12">
+        <v>2015</v>
+      </c>
+      <c r="F24" s="13">
+        <v>41616</v>
+      </c>
+      <c r="G24" s="13">
+        <v>42346</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="I24" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" s="17">
-        <v>2013</v>
-      </c>
-      <c r="E24" s="17">
-        <v>2015</v>
-      </c>
-      <c r="F24" s="18">
-        <v>41616</v>
-      </c>
-      <c r="G24" s="18">
-        <v>42346</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I24" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="J24" s="9">
+      <c r="J24" s="6">
         <v>23718.14</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="6">
         <v>23718.14</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1757,33 +1774,33 @@
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="12">
         <v>2013</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="12">
         <v>2014</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="13">
         <v>41466</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="13">
         <v>41665</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J25" s="9">
+        <v>68</v>
+      </c>
+      <c r="J25" s="6">
         <v>399828.18</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="6">
         <v>200000</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1792,28 +1809,28 @@
       <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="12">
         <v>2013</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="12">
         <v>2016</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="13">
         <v>41508</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="13">
         <v>42553</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J26" s="9">
+        <v>69</v>
+      </c>
+      <c r="J26" s="6">
         <v>289781.65999999997</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="6">
         <v>150722.66999999998</v>
       </c>
     </row>
@@ -1827,83 +1844,113 @@
       <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="12">
         <v>2013</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="12">
         <v>2014</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="13">
         <v>41465</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="13">
         <v>41829</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="6">
+        <v>19020.59</v>
+      </c>
+      <c r="K27" s="6">
+        <v>19020.59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="20">
+        <v>2015</v>
+      </c>
+      <c r="E28" s="20">
+        <v>2017</v>
+      </c>
+      <c r="F28" s="21">
+        <v>42583</v>
+      </c>
+      <c r="G28" s="21">
+        <v>43311</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="I28" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="9">
-        <v>19020.59</v>
-      </c>
-      <c r="K27" s="9">
-        <v>19020.59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="17">
-        <v>2015</v>
-      </c>
-      <c r="E28" s="17">
+      <c r="J28" s="22">
+        <v>2266180.4500000002</v>
+      </c>
+      <c r="K28" s="22">
+        <v>1982400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A29" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="27">
+        <v>2016</v>
+      </c>
+      <c r="E29" s="27">
         <v>2017</v>
       </c>
-      <c r="F28" s="18">
-        <v>42583</v>
-      </c>
-      <c r="G28" s="18">
-        <v>43311</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J28" s="9">
-        <v>2266180.4500000002</v>
-      </c>
-      <c r="K28" s="9">
-        <v>1982400</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="12">
-        <f>SUM(K2:K28)</f>
-        <v>9843804.870000001</v>
-      </c>
+      <c r="F29" s="28">
+        <v>42608</v>
+      </c>
+      <c r="G29" s="28">
+        <v>42972</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="K29" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1913,10 +1960,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1933,50 +1980,50 @@
     <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="16" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2">
         <v>2014</v>
@@ -1984,28 +2031,28 @@
       <c r="E2">
         <v>2015</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="15">
         <v>42318</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="15">
         <v>42683</v>
       </c>
       <c r="H2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" t="s">
         <v>95</v>
-      </c>
-      <c r="I2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="42" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -2019,23 +2066,23 @@
       <c r="E3">
         <v>2016</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="15">
         <v>42356</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="15">
         <v>42721</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" t="s">
         <v>98</v>
-      </c>
-      <c r="K3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="42" x14ac:dyDescent="0.2">
@@ -2043,10 +2090,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4">
         <v>2015</v>
@@ -2054,23 +2101,23 @@
       <c r="E4">
         <v>2015</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="15">
         <v>42278</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="15">
         <v>42369</v>
       </c>
       <c r="H4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" t="s">
         <v>101</v>
-      </c>
-      <c r="K4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2078,10 +2125,10 @@
         <v>294905</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>94</v>
+        <v>116</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>93</v>
       </c>
       <c r="D5">
         <v>2015</v>
@@ -2089,23 +2136,58 @@
       <c r="E5">
         <v>2015</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="15">
         <v>42064</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="15">
         <v>42459</v>
       </c>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K5" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="42" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6">
+        <v>2016</v>
+      </c>
+      <c r="E6">
+        <v>2017</v>
+      </c>
+      <c r="F6" s="15">
+        <v>42608</v>
+      </c>
+      <c r="G6" s="15">
+        <v>42972</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K6" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated gustavo's projects with faperj.
</commit_message>
<xml_diff>
--- a/database/projetos.xlsx
+++ b/database/projetos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13580" yWindow="8220" windowWidth="24740" windowHeight="12320" activeTab="1"/>
+    <workbookView xWindow="2420" yWindow="4080" windowWidth="24740" windowHeight="12320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="norberto" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="136">
   <si>
     <t>Tipo</t>
   </si>
@@ -419,6 +419,24 @@
   </si>
   <si>
     <t>Redução de custos operacionais e ambientais em sistema de geração termoelétrica</t>
+  </si>
+  <si>
+    <t>E-26/203.244/2016</t>
+  </si>
+  <si>
+    <t>Programa Jovem Cientista do Nosso Estado</t>
+  </si>
+  <si>
+    <t>30/09/2019</t>
+  </si>
+  <si>
+    <t>JCNE - Jovem Cientista do Nosso Estado 2016</t>
+  </si>
+  <si>
+    <t>Sistema de Alto Desempenho de Simulação de Escoamentos Multifásicos em Geometrias Complexas</t>
+  </si>
+  <si>
+    <t>75.600,00</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1642,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="56" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="42" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>37</v>
       </c>
@@ -1960,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2190,6 +2208,41 @@
         <v>126</v>
       </c>
     </row>
+    <row r="7" spans="1:11" ht="70" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7">
+        <v>2016</v>
+      </c>
+      <c r="E7">
+        <v>2016</v>
+      </c>
+      <c r="F7" s="15">
+        <v>42379</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J7" t="s">
+        <v>135</v>
+      </c>
+      <c r="K7" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated projects of Gustavo.
</commit_message>
<xml_diff>
--- a/database/projetos.xlsx
+++ b/database/projetos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="4080" windowWidth="24740" windowHeight="12320" activeTab="1"/>
+    <workbookView xWindow="11360" yWindow="8240" windowWidth="24740" windowHeight="12320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="norberto" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="143">
   <si>
     <t>Tipo</t>
   </si>
@@ -433,10 +433,31 @@
     <t>JCNE - Jovem Cientista do Nosso Estado 2016</t>
   </si>
   <si>
-    <t>Sistema de Alto Desempenho de Simulação de Escoamentos Multifásicos em Geometrias Complexas</t>
-  </si>
-  <si>
     <t>75.600,00</t>
+  </si>
+  <si>
+    <t>E-26/010.001642/2016</t>
+  </si>
+  <si>
+    <t>Sistema Multifásico de Arrefecimento de Componentes Eletrônicos</t>
+  </si>
+  <si>
+    <t>249.927,90</t>
+  </si>
+  <si>
+    <t>162.795,90</t>
+  </si>
+  <si>
+    <t>Apoio a Grupos Emergentes de Pesquisa no Estado do Rio de Janeiro 2016</t>
+  </si>
+  <si>
+    <t>Apoio a Grupos Emergentes</t>
+  </si>
+  <si>
+    <t>30/09/2018</t>
+  </si>
+  <si>
+    <t>Sistema de Alto Desempenho de Simulação de Escoamentos Multifásicos em Geometrias Complexas</t>
   </si>
 </sst>
 </file>
@@ -1978,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1995,7 +2016,7 @@
     <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="57.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="11" customFormat="1" ht="28" x14ac:dyDescent="0.2">
@@ -2222,7 +2243,7 @@
         <v>2016</v>
       </c>
       <c r="E7">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="F7" s="15">
         <v>42379</v>
@@ -2234,13 +2255,48 @@
         <v>133</v>
       </c>
       <c r="I7" t="s">
+        <v>142</v>
+      </c>
+      <c r="J7" t="s">
         <v>134</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="42" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>135</v>
       </c>
-      <c r="K7" t="s">
-        <v>135</v>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8">
+        <v>2016</v>
+      </c>
+      <c r="E8">
+        <v>2018</v>
+      </c>
+      <c r="F8" s="15">
+        <v>42379</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" t="s">
+        <v>136</v>
+      </c>
+      <c r="J8" t="s">
+        <v>137</v>
+      </c>
+      <c r="K8" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>